<commit_message>
Speed Highway: Car Textures
+ UnkEggViper2 -> njGetMatrix in pointers list
</commit_message>
<xml_diff>
--- a/AutoDemoPointers.xlsx
+++ b/AutoDemoPointers.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1B5BC9-5F94-4828-B6CD-96DDF89440A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0981355-520E-4088-8FB2-D8A85A6630FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19500" yWindow="1425" windowWidth="17925" windowHeight="9465" xr2:uid="{BF0A0D91-B89A-4FB4-ACC8-F22FBFD306B3}"/>
+    <workbookView xWindow="-19500" yWindow="1425" windowWidth="17715" windowHeight="9465" xr2:uid="{BF0A0D91-B89A-4FB4-ACC8-F22FBFD306B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Data List" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3356" uniqueCount="1859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3357" uniqueCount="1860">
   <si>
     <t>Big Endian</t>
   </si>
@@ -5593,9 +5593,6 @@
     <t>8C0587A0</t>
   </si>
   <si>
-    <t>UnkEggViper2</t>
-  </si>
-  <si>
     <t>8C5BE060</t>
   </si>
   <si>
@@ -5609,6 +5606,12 @@
   </si>
   <si>
     <t>8C6016AE</t>
+  </si>
+  <si>
+    <t>1807C8</t>
+  </si>
+  <si>
+    <t>njGetMatrix</t>
   </si>
 </sst>
 </file>
@@ -6234,8 +6237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491E3355-FE0C-4C06-9A33-67ABC97DABE2}">
   <dimension ref="A1:O503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F229" sqref="F229"/>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G448" sqref="G448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21092,7 +21095,7 @@
         <v>B0A85A8C</v>
       </c>
       <c r="E450" t="s">
-        <v>1853</v>
+        <v>1859</v>
       </c>
       <c r="F450" t="s">
         <v>1848</v>
@@ -21122,7 +21125,7 @@
         <v>B0A85A8C</v>
       </c>
       <c r="E451" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F451" t="s">
         <v>1849</v>
@@ -21152,7 +21155,7 @@
         <v>B0A85A8C</v>
       </c>
       <c r="E452" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="F452" t="s">
         <v>1850</v>
@@ -21793,6 +21796,9 @@
         <f t="shared" si="41"/>
         <v>74F25A8C</v>
       </c>
+      <c r="F496" t="s">
+        <v>1858</v>
+      </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
@@ -21844,10 +21850,10 @@
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B501" t="s">
         <v>1853</v>
-      </c>
-      <c r="B501" t="s">
-        <v>1854</v>
       </c>
       <c r="C501" t="str">
         <f t="shared" si="41"/>
@@ -21856,10 +21862,10 @@
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B502" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="C502" t="str">
         <f t="shared" si="41"/>
@@ -21868,10 +21874,10 @@
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="B503" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="C503" t="str">
         <f t="shared" si="41"/>

</xml_diff>